<commit_message>
Stacking and unstacking 3-level on data fromexcel file
</commit_message>
<xml_diff>
--- a/Resources/Products.xlsx
+++ b/Resources/Products.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>day</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>Nevada</t>
+  </si>
+  <si>
+    <t>Los Angles</t>
+  </si>
+  <si>
+    <t>Santa Monica</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Reno</t>
   </si>
 </sst>
 </file>
@@ -68,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -146,12 +158,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -161,19 +245,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -453,191 +537,349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>42736</v>
       </c>
-      <c r="B3" s="5">
-        <v>21</v>
-      </c>
-      <c r="C3" s="5">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B4" s="2">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2">
         <v>12</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E4" s="2">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2">
         <v>18</v>
       </c>
-      <c r="F3" s="5">
-        <v>15</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="I4" s="2">
+        <v>15</v>
+      </c>
+      <c r="J4" s="2">
         <v>12</v>
       </c>
+      <c r="K4" s="2">
+        <v>18</v>
+      </c>
+      <c r="L4" s="2">
+        <v>15</v>
+      </c>
+      <c r="M4" s="2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>42737</v>
       </c>
-      <c r="B4" s="5">
-        <v>22</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B5" s="2">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2">
         <v>14</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D5" s="2">
         <v>11</v>
       </c>
-      <c r="E4" s="5">
-        <v>22</v>
-      </c>
-      <c r="F4" s="5">
+      <c r="E5" s="2">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2">
         <v>14</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G5" s="2">
         <v>11</v>
       </c>
+      <c r="H5" s="2">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2">
+        <v>22</v>
+      </c>
+      <c r="L5" s="2">
+        <v>14</v>
+      </c>
+      <c r="M5" s="2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>42738</v>
       </c>
-      <c r="B5" s="5">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5">
-        <v>15</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="B6" s="2">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2">
         <v>10</v>
       </c>
-      <c r="E5" s="5">
-        <v>21</v>
-      </c>
-      <c r="F5" s="5">
-        <v>15</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="E6" s="2">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2">
         <v>10</v>
       </c>
+      <c r="H6" s="2">
+        <v>21</v>
+      </c>
+      <c r="I6" s="2">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2">
+        <v>10</v>
+      </c>
+      <c r="K6" s="2">
+        <v>21</v>
+      </c>
+      <c r="L6" s="2">
+        <v>15</v>
+      </c>
+      <c r="M6" s="2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>42739</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B7" s="2">
         <v>23</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="2">
         <v>13</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D7" s="2">
         <v>12</v>
       </c>
-      <c r="E6" s="5">
-        <v>22</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="E7" s="2">
+        <v>23</v>
+      </c>
+      <c r="F7" s="2">
         <v>13</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G7" s="2">
         <v>12</v>
       </c>
+      <c r="H7" s="2">
+        <v>22</v>
+      </c>
+      <c r="I7" s="2">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2">
+        <v>12</v>
+      </c>
+      <c r="K7" s="2">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2">
+        <v>13</v>
+      </c>
+      <c r="M7" s="2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>42740</v>
       </c>
-      <c r="B7" s="5">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B8" s="2">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2">
         <v>14</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D8" s="2">
         <v>10</v>
       </c>
-      <c r="E7" s="5">
-        <v>21</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E8" s="2">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2">
         <v>14</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G8" s="2">
         <v>10</v>
       </c>
+      <c r="H8" s="2">
+        <v>21</v>
+      </c>
+      <c r="I8" s="2">
+        <v>14</v>
+      </c>
+      <c r="J8" s="2">
+        <v>10</v>
+      </c>
+      <c r="K8" s="2">
+        <v>21</v>
+      </c>
+      <c r="L8" s="2">
+        <v>14</v>
+      </c>
+      <c r="M8" s="2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>42741</v>
       </c>
-      <c r="B8" s="6">
-        <v>22</v>
-      </c>
-      <c r="C8" s="6">
-        <v>15</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="B9" s="3">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3">
         <v>11</v>
       </c>
-      <c r="E8" s="6">
-        <v>22</v>
-      </c>
-      <c r="F8" s="6">
-        <v>15</v>
-      </c>
-      <c r="G8" s="6">
+      <c r="E9" s="3">
+        <v>22</v>
+      </c>
+      <c r="F9" s="3">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3">
+        <v>11</v>
+      </c>
+      <c r="H9" s="3">
+        <v>22</v>
+      </c>
+      <c r="I9" s="3">
+        <v>15</v>
+      </c>
+      <c r="J9" s="3">
+        <v>11</v>
+      </c>
+      <c r="K9" s="3">
+        <v>22</v>
+      </c>
+      <c r="L9" s="3">
+        <v>15</v>
+      </c>
+      <c r="M9" s="3">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="6">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="H1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>